<commit_message>
added new data from gummibears
</commit_message>
<xml_diff>
--- a/data/gummibears.xlsx
+++ b/data/gummibears.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/Documents/GitHub/jkruppa.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FACD302-BB31-DA4A-8FC6-3E6DA437EB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA5205D-09E8-234A-BC4F-71939453CA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1540" windowWidth="28800" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="27">
   <si>
     <t>m</t>
   </si>
@@ -638,8 +638,8 @@
   <dimension ref="A1:Q598"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A555" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D578" sqref="D578"/>
+      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H596" sqref="H596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -25794,7 +25794,7 @@
         <v>5</v>
       </c>
       <c r="K536" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L536" s="6" t="s">
         <v>1</v>
@@ -26080,7 +26080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="545" spans="1:14" ht="15.75" customHeight="1">
+    <row r="545" spans="1:15" ht="15.75" customHeight="1">
       <c r="A545" s="6">
         <v>2023</v>
       </c>
@@ -26112,7 +26112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="546" spans="1:14" ht="15.75" customHeight="1">
+    <row r="546" spans="1:15" ht="15.75" customHeight="1">
       <c r="A546" s="6">
         <v>2023</v>
       </c>
@@ -26144,7 +26144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="547" spans="1:14" ht="15.75" customHeight="1">
+    <row r="547" spans="1:15" ht="15.75" customHeight="1">
       <c r="A547" s="6">
         <v>2023</v>
       </c>
@@ -26176,7 +26176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="548" spans="1:14" ht="15.75" customHeight="1">
+    <row r="548" spans="1:15" ht="15.75" customHeight="1">
       <c r="A548" s="6">
         <v>2023</v>
       </c>
@@ -26208,7 +26208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="549" spans="1:14" ht="15.75" customHeight="1">
+    <row r="549" spans="1:15" ht="15.75" customHeight="1">
       <c r="A549" s="6">
         <v>2023</v>
       </c>
@@ -26240,7 +26240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="550" spans="1:14" ht="15.75" customHeight="1">
+    <row r="550" spans="1:15" ht="15.75" customHeight="1">
       <c r="A550" s="6">
         <v>2023</v>
       </c>
@@ -26272,7 +26272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="551" spans="1:14" ht="15.75" customHeight="1">
+    <row r="551" spans="1:15" ht="15.75" customHeight="1">
       <c r="A551" s="6">
         <v>2023</v>
       </c>
@@ -26304,7 +26304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="552" spans="1:14" ht="15.75" customHeight="1">
+    <row r="552" spans="1:15" ht="15.75" customHeight="1">
       <c r="A552" s="6">
         <v>2023</v>
       </c>
@@ -26336,7 +26336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="553" spans="1:14" ht="15.75" customHeight="1">
+    <row r="553" spans="1:15" ht="15.75" customHeight="1">
       <c r="A553" s="6">
         <v>2023</v>
       </c>
@@ -26368,7 +26368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="554" spans="1:14" ht="15.75" customHeight="1">
+    <row r="554" spans="1:15" ht="15.75" customHeight="1">
       <c r="A554" s="6">
         <v>2023</v>
       </c>
@@ -26400,7 +26400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="555" spans="1:14" ht="15.75" customHeight="1">
+    <row r="555" spans="1:15" ht="15.75" customHeight="1">
       <c r="A555" s="6">
         <v>2023</v>
       </c>
@@ -26432,7 +26432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="556" spans="1:14" ht="15.75" customHeight="1">
+    <row r="556" spans="1:15" ht="15.75" customHeight="1">
       <c r="A556" s="6">
         <v>2023</v>
       </c>
@@ -26475,8 +26475,11 @@
       <c r="N556">
         <v>172</v>
       </c>
-    </row>
-    <row r="557" spans="1:14" ht="15.75" customHeight="1">
+      <c r="O556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:15" ht="15.75" customHeight="1">
       <c r="A557" s="6">
         <v>2023</v>
       </c>
@@ -26508,7 +26511,7 @@
         <v>3</v>
       </c>
       <c r="K557" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L557" t="s">
         <v>1</v>
@@ -26519,8 +26522,11 @@
       <c r="N557">
         <v>160</v>
       </c>
-    </row>
-    <row r="558" spans="1:14" ht="15.75" customHeight="1">
+      <c r="O557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:15" ht="15.75" customHeight="1">
       <c r="A558" s="6">
         <v>2023</v>
       </c>
@@ -26563,8 +26569,11 @@
       <c r="N558">
         <v>173</v>
       </c>
-    </row>
-    <row r="559" spans="1:14" ht="15.75" customHeight="1">
+      <c r="O558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:15" ht="15.75" customHeight="1">
       <c r="A559" s="6">
         <v>2023</v>
       </c>
@@ -26607,8 +26616,11 @@
       <c r="N559">
         <v>159</v>
       </c>
-    </row>
-    <row r="560" spans="1:14" ht="15.75" customHeight="1">
+      <c r="O559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:15" ht="15.75" customHeight="1">
       <c r="A560" s="6">
         <v>2023</v>
       </c>
@@ -27153,7 +27165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="577" spans="1:10" ht="15.75" customHeight="1">
+    <row r="577" spans="1:15" ht="15.75" customHeight="1">
       <c r="A577" s="6">
         <v>2023</v>
       </c>
@@ -27185,172 +27197,736 @@
         <v>4</v>
       </c>
     </row>
-    <row r="578" spans="1:10" ht="15.75" customHeight="1">
+    <row r="578" spans="1:15" ht="15.75" customHeight="1">
       <c r="A578" s="6">
         <v>2023</v>
       </c>
       <c r="B578" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="579" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C578" s="6">
+        <v>0</v>
+      </c>
+      <c r="D578" s="6">
+        <v>1</v>
+      </c>
+      <c r="E578" s="6">
+        <v>2</v>
+      </c>
+      <c r="F578" s="6">
+        <v>2</v>
+      </c>
+      <c r="G578" s="6">
+        <v>1</v>
+      </c>
+      <c r="H578" s="6">
+        <v>1</v>
+      </c>
+      <c r="I578" s="6">
+        <v>7</v>
+      </c>
+      <c r="J578" s="6">
+        <v>5</v>
+      </c>
+      <c r="K578" t="s">
+        <v>3</v>
+      </c>
+      <c r="L578" t="s">
+        <v>1</v>
+      </c>
+      <c r="M578">
+        <v>12</v>
+      </c>
+      <c r="N578">
+        <v>158</v>
+      </c>
+      <c r="O578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:15" ht="15.75" customHeight="1">
       <c r="A579" s="6">
         <v>2023</v>
       </c>
       <c r="B579" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="580" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C579" s="6">
+        <v>0</v>
+      </c>
+      <c r="D579" s="6">
+        <v>1</v>
+      </c>
+      <c r="E579" s="6">
+        <v>4</v>
+      </c>
+      <c r="F579" s="6">
+        <v>1</v>
+      </c>
+      <c r="G579" s="6">
+        <v>1</v>
+      </c>
+      <c r="H579" s="6">
+        <v>1</v>
+      </c>
+      <c r="I579">
+        <v>8</v>
+      </c>
+      <c r="J579" s="6">
+        <v>5</v>
+      </c>
+      <c r="K579" t="s">
+        <v>3</v>
+      </c>
+      <c r="L579" t="s">
+        <v>1</v>
+      </c>
+      <c r="M579">
+        <v>12</v>
+      </c>
+      <c r="N579">
+        <v>158</v>
+      </c>
+      <c r="O579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:15" ht="15.75" customHeight="1">
       <c r="A580" s="6">
         <v>2023</v>
       </c>
       <c r="B580" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="581" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C580" s="6">
+        <v>1</v>
+      </c>
+      <c r="D580" s="6">
+        <v>1</v>
+      </c>
+      <c r="E580" s="6">
+        <v>0</v>
+      </c>
+      <c r="F580" s="6">
+        <v>2</v>
+      </c>
+      <c r="G580" s="6">
+        <v>1</v>
+      </c>
+      <c r="H580" s="6">
+        <v>2</v>
+      </c>
+      <c r="I580">
+        <v>7</v>
+      </c>
+      <c r="J580" s="6">
+        <v>5</v>
+      </c>
+      <c r="K580" t="s">
+        <v>3</v>
+      </c>
+      <c r="L580" t="s">
+        <v>1</v>
+      </c>
+      <c r="M580">
+        <v>12</v>
+      </c>
+      <c r="N580">
+        <v>156</v>
+      </c>
+      <c r="O580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:15" ht="15.75" customHeight="1">
       <c r="A581" s="6">
         <v>2023</v>
       </c>
       <c r="B581" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="582" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C581" s="6">
+        <v>0</v>
+      </c>
+      <c r="D581" s="6">
+        <v>3</v>
+      </c>
+      <c r="E581" s="6">
+        <v>2</v>
+      </c>
+      <c r="F581" s="6">
+        <v>1</v>
+      </c>
+      <c r="G581" s="6">
+        <v>1</v>
+      </c>
+      <c r="H581" s="6">
+        <v>0</v>
+      </c>
+      <c r="I581">
+        <v>7</v>
+      </c>
+      <c r="J581" s="6">
+        <v>4</v>
+      </c>
+      <c r="K581" t="s">
+        <v>3</v>
+      </c>
+      <c r="L581" t="s">
+        <v>1</v>
+      </c>
+      <c r="M581">
+        <v>12</v>
+      </c>
+      <c r="N581">
+        <v>158</v>
+      </c>
+      <c r="O581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:15" ht="15.75" customHeight="1">
       <c r="A582" s="6">
         <v>2023</v>
       </c>
       <c r="B582" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="583" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C582" s="6">
+        <v>2</v>
+      </c>
+      <c r="D582" s="6">
+        <v>2</v>
+      </c>
+      <c r="E582" s="6">
+        <v>2</v>
+      </c>
+      <c r="F582" s="6">
+        <v>0</v>
+      </c>
+      <c r="G582" s="6">
+        <v>0</v>
+      </c>
+      <c r="H582" s="6">
+        <v>1</v>
+      </c>
+      <c r="I582">
+        <v>7</v>
+      </c>
+      <c r="J582" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="583" spans="1:15" ht="15.75" customHeight="1">
       <c r="A583" s="6">
         <v>2023</v>
       </c>
       <c r="B583" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="584" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C583" s="6">
+        <v>1</v>
+      </c>
+      <c r="D583" s="6">
+        <v>1</v>
+      </c>
+      <c r="E583" s="6">
+        <v>1</v>
+      </c>
+      <c r="F583" s="6">
+        <v>1</v>
+      </c>
+      <c r="G583" s="6">
+        <v>2</v>
+      </c>
+      <c r="H583" s="6">
+        <v>3</v>
+      </c>
+      <c r="I583">
+        <v>9</v>
+      </c>
+      <c r="J583" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="584" spans="1:15" ht="15.75" customHeight="1">
       <c r="A584" s="6">
         <v>2023</v>
       </c>
       <c r="B584" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="585" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C584" s="6">
+        <v>2</v>
+      </c>
+      <c r="D584" s="6">
+        <v>0</v>
+      </c>
+      <c r="E584" s="6">
+        <v>1</v>
+      </c>
+      <c r="F584" s="6">
+        <v>3</v>
+      </c>
+      <c r="G584" s="6">
+        <v>2</v>
+      </c>
+      <c r="H584" s="6">
+        <v>0</v>
+      </c>
+      <c r="I584">
+        <v>8</v>
+      </c>
+      <c r="J584" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="585" spans="1:15" ht="15.75" customHeight="1">
       <c r="A585" s="6">
         <v>2023</v>
       </c>
       <c r="B585" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="586" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C585" s="6">
+        <v>1</v>
+      </c>
+      <c r="D585" s="6">
+        <v>1</v>
+      </c>
+      <c r="E585" s="6">
+        <v>1</v>
+      </c>
+      <c r="F585" s="6">
+        <v>3</v>
+      </c>
+      <c r="G585" s="6">
+        <v>1</v>
+      </c>
+      <c r="H585" s="6">
+        <v>1</v>
+      </c>
+      <c r="I585">
+        <v>8</v>
+      </c>
+      <c r="J585" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="586" spans="1:15" ht="15.75" customHeight="1">
       <c r="A586" s="6">
         <v>2023</v>
       </c>
       <c r="B586" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="587" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C586" s="6">
+        <v>1</v>
+      </c>
+      <c r="D586" s="6">
+        <v>0</v>
+      </c>
+      <c r="E586" s="6">
+        <v>2</v>
+      </c>
+      <c r="F586" s="6">
+        <v>1</v>
+      </c>
+      <c r="G586" s="6">
+        <v>3</v>
+      </c>
+      <c r="H586" s="6">
+        <v>1</v>
+      </c>
+      <c r="I586">
+        <v>8</v>
+      </c>
+      <c r="J586" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="587" spans="1:15" ht="15.75" customHeight="1">
       <c r="A587" s="6">
         <v>2023</v>
       </c>
       <c r="B587" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="588" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C587" s="6">
+        <v>0</v>
+      </c>
+      <c r="D587" s="6">
+        <v>1</v>
+      </c>
+      <c r="E587" s="6">
+        <v>1</v>
+      </c>
+      <c r="F587" s="6">
+        <v>3</v>
+      </c>
+      <c r="G587" s="6">
+        <v>2</v>
+      </c>
+      <c r="H587" s="6">
+        <v>0</v>
+      </c>
+      <c r="I587">
+        <v>7</v>
+      </c>
+      <c r="J587" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="588" spans="1:15" ht="15.75" customHeight="1">
       <c r="A588" s="6">
         <v>2023</v>
       </c>
       <c r="B588" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="589" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C588" s="6">
+        <v>1</v>
+      </c>
+      <c r="D588" s="6">
+        <v>2</v>
+      </c>
+      <c r="E588" s="6">
+        <v>2</v>
+      </c>
+      <c r="F588" s="6">
+        <v>3</v>
+      </c>
+      <c r="G588" s="6">
+        <v>1</v>
+      </c>
+      <c r="H588" s="6">
+        <v>1</v>
+      </c>
+      <c r="I588">
+        <v>10</v>
+      </c>
+      <c r="J588" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="589" spans="1:15" ht="15.75" customHeight="1">
       <c r="A589" s="6">
         <v>2023</v>
       </c>
       <c r="B589" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="590" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C589" s="6">
+        <v>3</v>
+      </c>
+      <c r="D589" s="6">
+        <v>4</v>
+      </c>
+      <c r="E589" s="6">
+        <v>1</v>
+      </c>
+      <c r="F589" s="6">
+        <v>0</v>
+      </c>
+      <c r="G589" s="6">
+        <v>0</v>
+      </c>
+      <c r="H589" s="6">
+        <v>2</v>
+      </c>
+      <c r="I589">
+        <v>10</v>
+      </c>
+      <c r="J589" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="590" spans="1:15" ht="15.75" customHeight="1">
       <c r="A590" s="6">
         <v>2023</v>
       </c>
       <c r="B590" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="591" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C590" s="6">
+        <v>1</v>
+      </c>
+      <c r="D590" s="6">
+        <v>1</v>
+      </c>
+      <c r="E590" s="6">
+        <v>1</v>
+      </c>
+      <c r="F590" s="6">
+        <v>2</v>
+      </c>
+      <c r="G590" s="6">
+        <v>2</v>
+      </c>
+      <c r="H590" s="6">
+        <v>1</v>
+      </c>
+      <c r="I590">
+        <v>8</v>
+      </c>
+      <c r="J590" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="591" spans="1:15" ht="15.75" customHeight="1">
       <c r="A591" s="6">
         <v>2023</v>
       </c>
       <c r="B591" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="592" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C591" s="6">
+        <v>2</v>
+      </c>
+      <c r="D591" s="6">
+        <v>1</v>
+      </c>
+      <c r="E591" s="6">
+        <v>1</v>
+      </c>
+      <c r="F591" s="6">
+        <v>1</v>
+      </c>
+      <c r="G591" s="6">
+        <v>2</v>
+      </c>
+      <c r="H591" s="6">
+        <v>3</v>
+      </c>
+      <c r="I591">
+        <v>10</v>
+      </c>
+      <c r="J591" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="592" spans="1:15" ht="15.75" customHeight="1">
       <c r="A592" s="6">
         <v>2023</v>
       </c>
       <c r="B592" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="593" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C592" s="6">
+        <v>2</v>
+      </c>
+      <c r="D592" s="6">
+        <v>1</v>
+      </c>
+      <c r="E592" s="6">
+        <v>1</v>
+      </c>
+      <c r="F592" s="6">
+        <v>3</v>
+      </c>
+      <c r="G592" s="6">
+        <v>1</v>
+      </c>
+      <c r="H592" s="6">
+        <v>1</v>
+      </c>
+      <c r="I592">
+        <v>9</v>
+      </c>
+      <c r="J592" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="593" spans="1:10" ht="15.75" customHeight="1">
       <c r="A593" s="6">
         <v>2023</v>
       </c>
       <c r="B593" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="594" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C593" s="6">
+        <v>0</v>
+      </c>
+      <c r="D593" s="6">
+        <v>2</v>
+      </c>
+      <c r="E593" s="6">
+        <v>1</v>
+      </c>
+      <c r="F593" s="6">
+        <v>2</v>
+      </c>
+      <c r="G593" s="6">
+        <v>4</v>
+      </c>
+      <c r="H593" s="6">
+        <v>0</v>
+      </c>
+      <c r="I593">
+        <v>9</v>
+      </c>
+      <c r="J593" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10" ht="15.75" customHeight="1">
       <c r="A594" s="6">
         <v>2023</v>
       </c>
       <c r="B594" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="595" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C594" s="6">
+        <v>1</v>
+      </c>
+      <c r="D594" s="6">
+        <v>2</v>
+      </c>
+      <c r="E594" s="6">
+        <v>0</v>
+      </c>
+      <c r="F594" s="6">
+        <v>0</v>
+      </c>
+      <c r="G594" s="6">
+        <v>2</v>
+      </c>
+      <c r="H594" s="6">
+        <v>3</v>
+      </c>
+      <c r="I594">
+        <v>9</v>
+      </c>
+      <c r="J594" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10" ht="15.75" customHeight="1">
       <c r="A595" s="6">
         <v>2023</v>
       </c>
       <c r="B595" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="596" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C595" s="6">
+        <v>0</v>
+      </c>
+      <c r="D595" s="6">
+        <v>3</v>
+      </c>
+      <c r="E595" s="6">
+        <v>2</v>
+      </c>
+      <c r="F595" s="6">
+        <v>1</v>
+      </c>
+      <c r="G595" s="6">
+        <v>2</v>
+      </c>
+      <c r="H595" s="6">
+        <v>0</v>
+      </c>
+      <c r="I595">
+        <v>8</v>
+      </c>
+      <c r="J595" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10" ht="15.75" customHeight="1">
       <c r="A596" s="6">
         <v>2023</v>
       </c>
       <c r="B596" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="597" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C596" s="6">
+        <v>0</v>
+      </c>
+      <c r="D596">
+        <v>0</v>
+      </c>
+      <c r="E596">
+        <v>0</v>
+      </c>
+      <c r="F596">
+        <v>4</v>
+      </c>
+      <c r="G596">
+        <v>2</v>
+      </c>
+      <c r="H596">
+        <v>2</v>
+      </c>
+      <c r="I596">
+        <v>8</v>
+      </c>
+      <c r="J596" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10" ht="15.75" customHeight="1">
       <c r="A597" s="6">
         <v>2023</v>
       </c>
       <c r="B597" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="598" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C597" s="6">
+        <v>0</v>
+      </c>
+      <c r="D597">
+        <v>0</v>
+      </c>
+      <c r="E597">
+        <v>1</v>
+      </c>
+      <c r="F597">
+        <v>2</v>
+      </c>
+      <c r="G597">
+        <v>4</v>
+      </c>
+      <c r="H597">
+        <v>1</v>
+      </c>
+      <c r="I597">
+        <v>8</v>
+      </c>
+      <c r="J597" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10" ht="15.75" customHeight="1">
       <c r="A598" s="6">
         <v>2023</v>
       </c>
       <c r="B598" s="6" t="s">
         <v>26</v>
+      </c>
+      <c r="C598" s="6">
+        <v>0</v>
+      </c>
+      <c r="D598">
+        <v>0</v>
+      </c>
+      <c r="E598">
+        <v>4</v>
+      </c>
+      <c r="F598">
+        <v>2</v>
+      </c>
+      <c r="G598">
+        <v>1</v>
+      </c>
+      <c r="H598">
+        <v>1</v>
+      </c>
+      <c r="I598">
+        <v>8</v>
+      </c>
+      <c r="J598" s="6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugs in gumi bears and our world in data
</commit_message>
<xml_diff>
--- a/data/gummibears.xlsx
+++ b/data/gummibears.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/Documents/GitHub/jkruppa.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3F3221-D0A7-E741-8A93-9AB0DB06119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E19620A0-B00C-6344-B5CE-99AA568D56BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1540" windowWidth="28800" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="27">
   <si>
     <t>m</t>
   </si>
@@ -635,11 +635,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q545"/>
+  <dimension ref="A1:Q598"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I556" sqref="I556"/>
+      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H596" sqref="H596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -25867,40 +25867,25 @@
         <v>0</v>
       </c>
       <c r="D538" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E538" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F538" s="6">
         <v>1</v>
       </c>
       <c r="G538" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H538" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I538" s="6">
         <v>8</v>
       </c>
       <c r="J538" s="6">
-        <v>5</v>
-      </c>
-      <c r="K538" t="s">
-        <v>5</v>
-      </c>
-      <c r="L538" t="s">
-        <v>1</v>
-      </c>
-      <c r="M538">
-        <v>14</v>
-      </c>
-      <c r="N538">
-        <v>172</v>
-      </c>
-      <c r="O538">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="539" spans="1:16" ht="15.75" customHeight="1">
@@ -25911,10 +25896,10 @@
         <v>26</v>
       </c>
       <c r="C539" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D539" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E539" s="6">
         <v>1</v>
@@ -25923,31 +25908,16 @@
         <v>0</v>
       </c>
       <c r="G539" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H539" s="6">
         <v>0</v>
       </c>
       <c r="I539" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J539" s="6">
-        <v>3</v>
-      </c>
-      <c r="K539" t="s">
-        <v>3</v>
-      </c>
-      <c r="L539" t="s">
-        <v>1</v>
-      </c>
-      <c r="M539">
-        <v>13</v>
-      </c>
-      <c r="N539">
-        <v>160</v>
-      </c>
-      <c r="O539">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="540" spans="1:16" ht="15.75" customHeight="1">
@@ -25958,43 +25928,28 @@
         <v>26</v>
       </c>
       <c r="C540" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D540" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E540" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F540" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G540" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H540" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I540" s="6">
         <v>8</v>
       </c>
       <c r="J540" s="6">
         <v>5</v>
-      </c>
-      <c r="K540" t="s">
-        <v>8</v>
-      </c>
-      <c r="L540" t="s">
-        <v>1</v>
-      </c>
-      <c r="M540">
-        <v>14</v>
-      </c>
-      <c r="N540">
-        <v>173</v>
-      </c>
-      <c r="O540">
-        <v>0</v>
       </c>
     </row>
     <row r="541" spans="1:16" ht="15.75" customHeight="1">
@@ -26008,40 +25963,25 @@
         <v>1</v>
       </c>
       <c r="D541" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E541" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F541" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G541" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H541" s="6">
         <v>2</v>
       </c>
       <c r="I541" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J541" s="6">
         <v>5</v>
-      </c>
-      <c r="K541" t="s">
-        <v>21</v>
-      </c>
-      <c r="L541" t="s">
-        <v>1</v>
-      </c>
-      <c r="M541">
-        <v>11</v>
-      </c>
-      <c r="N541">
-        <v>159</v>
-      </c>
-      <c r="O541">
-        <v>0</v>
       </c>
     </row>
     <row r="542" spans="1:16" ht="15.75" customHeight="1">
@@ -26052,16 +25992,16 @@
         <v>26</v>
       </c>
       <c r="C542" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D542" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E542" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F542" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G542" s="6">
         <v>1</v>
@@ -26070,25 +26010,10 @@
         <v>1</v>
       </c>
       <c r="I542" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J542" s="6">
         <v>5</v>
-      </c>
-      <c r="K542" t="s">
-        <v>3</v>
-      </c>
-      <c r="L542" t="s">
-        <v>1</v>
-      </c>
-      <c r="M542">
-        <v>12</v>
-      </c>
-      <c r="N542">
-        <v>158</v>
-      </c>
-      <c r="O542">
-        <v>0</v>
       </c>
     </row>
     <row r="543" spans="1:16" ht="15.75" customHeight="1">
@@ -26099,43 +26024,28 @@
         <v>26</v>
       </c>
       <c r="C543" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D543" s="6">
         <v>1</v>
       </c>
       <c r="E543" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F543" s="6">
         <v>1</v>
       </c>
       <c r="G543" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H543" s="6">
-        <v>1</v>
-      </c>
-      <c r="I543">
+        <v>2</v>
+      </c>
+      <c r="I543" s="6">
         <v>8</v>
       </c>
       <c r="J543" s="6">
         <v>5</v>
-      </c>
-      <c r="K543" t="s">
-        <v>3</v>
-      </c>
-      <c r="L543" t="s">
-        <v>1</v>
-      </c>
-      <c r="M543">
-        <v>12</v>
-      </c>
-      <c r="N543">
-        <v>158</v>
-      </c>
-      <c r="O543">
-        <v>0</v>
       </c>
     </row>
     <row r="544" spans="1:16" ht="15.75" customHeight="1">
@@ -26146,43 +26056,28 @@
         <v>26</v>
       </c>
       <c r="C544" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D544" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E544" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F544" s="6">
         <v>2</v>
       </c>
       <c r="G544" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H544" s="6">
-        <v>2</v>
-      </c>
-      <c r="I544">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="I544" s="6">
+        <v>8</v>
       </c>
       <c r="J544" s="6">
         <v>5</v>
-      </c>
-      <c r="K544" t="s">
-        <v>3</v>
-      </c>
-      <c r="L544" t="s">
-        <v>1</v>
-      </c>
-      <c r="M544">
-        <v>12</v>
-      </c>
-      <c r="N544">
-        <v>156</v>
-      </c>
-      <c r="O544">
-        <v>0</v>
       </c>
     </row>
     <row r="545" spans="1:15" ht="15.75" customHeight="1">
@@ -26193,43 +26088,1845 @@
         <v>26</v>
       </c>
       <c r="C545" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D545" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E545" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F545" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G545" s="6">
-        <v>1</v>
-      </c>
-      <c r="H545" s="6">
-        <v>0</v>
-      </c>
-      <c r="I545">
+        <v>2</v>
+      </c>
+      <c r="H545">
+        <v>0</v>
+      </c>
+      <c r="I545" s="6">
         <v>7</v>
       </c>
       <c r="J545" s="6">
         <v>4</v>
       </c>
-      <c r="K545" t="s">
-        <v>3</v>
-      </c>
-      <c r="L545" t="s">
-        <v>1</v>
-      </c>
-      <c r="M545">
+    </row>
+    <row r="546" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A546" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B546" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C546" s="6">
+        <v>0</v>
+      </c>
+      <c r="D546" s="6">
+        <v>1</v>
+      </c>
+      <c r="E546" s="6">
+        <v>2</v>
+      </c>
+      <c r="F546" s="6">
+        <v>3</v>
+      </c>
+      <c r="G546" s="6">
+        <v>2</v>
+      </c>
+      <c r="H546" s="6">
+        <v>0</v>
+      </c>
+      <c r="I546" s="6">
+        <v>8</v>
+      </c>
+      <c r="J546" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="547" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A547" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B547" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C547" s="6">
+        <v>3</v>
+      </c>
+      <c r="D547" s="6">
+        <v>0</v>
+      </c>
+      <c r="E547" s="6">
+        <v>2</v>
+      </c>
+      <c r="F547" s="6">
+        <v>1</v>
+      </c>
+      <c r="G547" s="6">
+        <v>1</v>
+      </c>
+      <c r="H547" s="6">
+        <v>1</v>
+      </c>
+      <c r="I547" s="6">
+        <v>8</v>
+      </c>
+      <c r="J547" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="548" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A548" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B548" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C548" s="6">
+        <v>1</v>
+      </c>
+      <c r="D548" s="6">
+        <v>0</v>
+      </c>
+      <c r="E548" s="6">
+        <v>0</v>
+      </c>
+      <c r="F548" s="6">
+        <v>4</v>
+      </c>
+      <c r="G548" s="6">
+        <v>2</v>
+      </c>
+      <c r="H548" s="6">
+        <v>1</v>
+      </c>
+      <c r="I548" s="6">
+        <v>8</v>
+      </c>
+      <c r="J548" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="549" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A549" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B549" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C549" s="6">
+        <v>3</v>
+      </c>
+      <c r="D549" s="6">
+        <v>2</v>
+      </c>
+      <c r="E549" s="6">
+        <v>2</v>
+      </c>
+      <c r="F549" s="6">
+        <v>1</v>
+      </c>
+      <c r="G549" s="6">
+        <v>0</v>
+      </c>
+      <c r="H549" s="6">
+        <v>0</v>
+      </c>
+      <c r="I549" s="6">
+        <v>8</v>
+      </c>
+      <c r="J549" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="550" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A550" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B550" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C550" s="6">
+        <v>1</v>
+      </c>
+      <c r="D550" s="6">
+        <v>2</v>
+      </c>
+      <c r="E550" s="6">
+        <v>1</v>
+      </c>
+      <c r="F550" s="6">
+        <v>2</v>
+      </c>
+      <c r="G550" s="6">
+        <v>2</v>
+      </c>
+      <c r="H550" s="6">
+        <v>0</v>
+      </c>
+      <c r="I550" s="6">
+        <v>8</v>
+      </c>
+      <c r="J550" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="551" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A551" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B551" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C551" s="6">
+        <v>3</v>
+      </c>
+      <c r="D551" s="6">
+        <v>1</v>
+      </c>
+      <c r="E551" s="6">
+        <v>0</v>
+      </c>
+      <c r="F551" s="6">
+        <v>0</v>
+      </c>
+      <c r="G551" s="6">
+        <v>2</v>
+      </c>
+      <c r="H551" s="6">
+        <v>2</v>
+      </c>
+      <c r="I551" s="6">
+        <v>8</v>
+      </c>
+      <c r="J551" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="552" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A552" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B552" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C552" s="6">
+        <v>2</v>
+      </c>
+      <c r="D552" s="6">
+        <v>1</v>
+      </c>
+      <c r="E552" s="6">
+        <v>1</v>
+      </c>
+      <c r="F552" s="6">
+        <v>1</v>
+      </c>
+      <c r="G552" s="6">
+        <v>2</v>
+      </c>
+      <c r="H552" s="6">
+        <v>1</v>
+      </c>
+      <c r="I552" s="6">
+        <v>8</v>
+      </c>
+      <c r="J552" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="553" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A553" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B553" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C553" s="6">
+        <v>1</v>
+      </c>
+      <c r="D553" s="6">
+        <v>3</v>
+      </c>
+      <c r="E553" s="6">
+        <v>2</v>
+      </c>
+      <c r="F553" s="6">
+        <v>2</v>
+      </c>
+      <c r="G553" s="6">
+        <v>0</v>
+      </c>
+      <c r="H553" s="6">
+        <v>0</v>
+      </c>
+      <c r="I553" s="6">
+        <v>8</v>
+      </c>
+      <c r="J553" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="554" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A554" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B554" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C554" s="6">
+        <v>2</v>
+      </c>
+      <c r="D554" s="6">
+        <v>1</v>
+      </c>
+      <c r="E554" s="6">
+        <v>1</v>
+      </c>
+      <c r="F554" s="6">
+        <v>1</v>
+      </c>
+      <c r="G554" s="6">
+        <v>2</v>
+      </c>
+      <c r="H554" s="6">
+        <v>2</v>
+      </c>
+      <c r="I554" s="6">
+        <v>9</v>
+      </c>
+      <c r="J554" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="555" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A555" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B555" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C555" s="6">
+        <v>1</v>
+      </c>
+      <c r="D555" s="6">
+        <v>0</v>
+      </c>
+      <c r="E555" s="6">
+        <v>3</v>
+      </c>
+      <c r="F555" s="6">
+        <v>3</v>
+      </c>
+      <c r="G555" s="6">
+        <v>1</v>
+      </c>
+      <c r="H555" s="6">
+        <v>1</v>
+      </c>
+      <c r="I555" s="6">
+        <v>9</v>
+      </c>
+      <c r="J555" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="556" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A556" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B556" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C556" s="6">
+        <v>0</v>
+      </c>
+      <c r="D556" s="6">
+        <v>1</v>
+      </c>
+      <c r="E556" s="6">
+        <v>1</v>
+      </c>
+      <c r="F556" s="6">
+        <v>1</v>
+      </c>
+      <c r="G556" s="6">
+        <v>3</v>
+      </c>
+      <c r="H556" s="6">
+        <v>2</v>
+      </c>
+      <c r="I556" s="6">
+        <v>8</v>
+      </c>
+      <c r="J556" s="6">
+        <v>5</v>
+      </c>
+      <c r="K556" t="s">
+        <v>5</v>
+      </c>
+      <c r="L556" t="s">
+        <v>1</v>
+      </c>
+      <c r="M556">
+        <v>14</v>
+      </c>
+      <c r="N556">
+        <v>172</v>
+      </c>
+      <c r="O556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A557" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B557" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C557" s="6">
+        <v>0</v>
+      </c>
+      <c r="D557" s="6">
+        <v>4</v>
+      </c>
+      <c r="E557" s="6">
+        <v>1</v>
+      </c>
+      <c r="F557" s="6">
+        <v>0</v>
+      </c>
+      <c r="G557" s="6">
+        <v>2</v>
+      </c>
+      <c r="H557" s="6">
+        <v>0</v>
+      </c>
+      <c r="I557" s="6">
+        <v>7</v>
+      </c>
+      <c r="J557" s="6">
+        <v>3</v>
+      </c>
+      <c r="K557" t="s">
+        <v>3</v>
+      </c>
+      <c r="L557" t="s">
+        <v>1</v>
+      </c>
+      <c r="M557">
+        <v>13</v>
+      </c>
+      <c r="N557">
+        <v>160</v>
+      </c>
+      <c r="O557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A558" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B558" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C558" s="6">
+        <v>1</v>
+      </c>
+      <c r="D558" s="6">
+        <v>3</v>
+      </c>
+      <c r="E558" s="6">
+        <v>0</v>
+      </c>
+      <c r="F558" s="6">
+        <v>1</v>
+      </c>
+      <c r="G558" s="6">
+        <v>1</v>
+      </c>
+      <c r="H558" s="6">
+        <v>2</v>
+      </c>
+      <c r="I558" s="6">
+        <v>8</v>
+      </c>
+      <c r="J558" s="6">
+        <v>5</v>
+      </c>
+      <c r="K558" t="s">
+        <v>8</v>
+      </c>
+      <c r="L558" t="s">
+        <v>1</v>
+      </c>
+      <c r="M558">
+        <v>14</v>
+      </c>
+      <c r="N558">
+        <v>173</v>
+      </c>
+      <c r="O558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A559" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B559" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C559" s="6">
+        <v>1</v>
+      </c>
+      <c r="D559" s="6">
+        <v>1</v>
+      </c>
+      <c r="E559" s="6">
+        <v>2</v>
+      </c>
+      <c r="F559" s="6">
+        <v>1</v>
+      </c>
+      <c r="G559" s="6">
+        <v>0</v>
+      </c>
+      <c r="H559" s="6">
+        <v>2</v>
+      </c>
+      <c r="I559" s="6">
+        <v>7</v>
+      </c>
+      <c r="J559" s="6">
+        <v>5</v>
+      </c>
+      <c r="K559" t="s">
+        <v>21</v>
+      </c>
+      <c r="L559" t="s">
+        <v>1</v>
+      </c>
+      <c r="M559">
+        <v>11</v>
+      </c>
+      <c r="N559">
+        <v>159</v>
+      </c>
+      <c r="O559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A560" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B560" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C560" s="6">
+        <v>0</v>
+      </c>
+      <c r="D560" s="6">
+        <v>1</v>
+      </c>
+      <c r="E560" s="6">
+        <v>5</v>
+      </c>
+      <c r="F560" s="6">
+        <v>1</v>
+      </c>
+      <c r="G560" s="6">
+        <v>0</v>
+      </c>
+      <c r="H560" s="6">
+        <v>1</v>
+      </c>
+      <c r="I560" s="6">
+        <v>8</v>
+      </c>
+      <c r="J560" s="6">
+        <v>4</v>
+      </c>
+      <c r="K560" s="6"/>
+    </row>
+    <row r="561" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A561" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B561" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C561" s="6">
+        <v>3</v>
+      </c>
+      <c r="D561" s="6">
+        <v>2</v>
+      </c>
+      <c r="E561" s="6">
+        <v>0</v>
+      </c>
+      <c r="F561" s="6">
+        <v>2</v>
+      </c>
+      <c r="G561" s="6">
+        <v>0</v>
+      </c>
+      <c r="H561" s="6">
+        <v>1</v>
+      </c>
+      <c r="I561" s="6">
+        <v>8</v>
+      </c>
+      <c r="J561" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="562" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A562" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B562" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C562" s="6">
+        <v>2</v>
+      </c>
+      <c r="D562" s="6">
+        <v>2</v>
+      </c>
+      <c r="E562" s="6">
+        <v>1</v>
+      </c>
+      <c r="F562" s="6">
+        <v>0</v>
+      </c>
+      <c r="G562" s="6">
+        <v>1</v>
+      </c>
+      <c r="H562" s="6">
+        <v>2</v>
+      </c>
+      <c r="I562" s="6">
+        <v>8</v>
+      </c>
+      <c r="J562" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="563" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A563" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B563" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C563" s="6">
+        <v>1</v>
+      </c>
+      <c r="D563" s="6">
+        <v>0</v>
+      </c>
+      <c r="E563" s="6">
+        <v>0</v>
+      </c>
+      <c r="F563" s="6">
+        <v>1</v>
+      </c>
+      <c r="G563" s="6">
+        <v>3</v>
+      </c>
+      <c r="H563" s="6">
+        <v>3</v>
+      </c>
+      <c r="I563" s="6">
+        <v>8</v>
+      </c>
+      <c r="J563" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="564" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A564" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B564" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C564" s="6">
+        <v>1</v>
+      </c>
+      <c r="D564" s="6">
+        <v>0</v>
+      </c>
+      <c r="E564" s="6">
+        <v>0</v>
+      </c>
+      <c r="F564" s="6">
+        <v>4</v>
+      </c>
+      <c r="G564" s="6">
+        <v>2</v>
+      </c>
+      <c r="H564" s="6">
+        <v>3</v>
+      </c>
+      <c r="I564" s="6">
+        <v>10</v>
+      </c>
+      <c r="J564" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="565" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A565" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B565" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C565" s="6">
+        <v>1</v>
+      </c>
+      <c r="D565" s="6">
+        <v>2</v>
+      </c>
+      <c r="E565" s="6">
+        <v>2</v>
+      </c>
+      <c r="F565" s="6">
+        <v>0</v>
+      </c>
+      <c r="G565" s="6">
+        <v>1</v>
+      </c>
+      <c r="H565" s="6">
+        <v>2</v>
+      </c>
+      <c r="I565" s="6">
+        <v>8</v>
+      </c>
+      <c r="J565" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="566" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A566" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B566" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C566" s="6">
+        <v>2</v>
+      </c>
+      <c r="D566" s="6">
+        <v>0</v>
+      </c>
+      <c r="E566" s="6">
+        <v>1</v>
+      </c>
+      <c r="F566" s="6">
+        <v>2</v>
+      </c>
+      <c r="G566" s="6">
+        <v>2</v>
+      </c>
+      <c r="H566" s="6">
+        <v>0</v>
+      </c>
+      <c r="I566" s="6">
+        <v>7</v>
+      </c>
+      <c r="J566" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="567" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A567" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B567" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C567" s="6">
+        <v>0</v>
+      </c>
+      <c r="D567" s="6">
+        <v>2</v>
+      </c>
+      <c r="E567" s="6">
+        <v>2</v>
+      </c>
+      <c r="F567" s="6">
+        <v>1</v>
+      </c>
+      <c r="G567" s="6">
+        <v>0</v>
+      </c>
+      <c r="H567" s="6">
+        <v>2</v>
+      </c>
+      <c r="I567" s="6">
+        <v>7</v>
+      </c>
+      <c r="J567" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="568" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A568" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B568" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C568" s="6">
+        <v>2</v>
+      </c>
+      <c r="D568" s="6">
+        <v>0</v>
+      </c>
+      <c r="E568" s="6">
+        <v>2</v>
+      </c>
+      <c r="F568" s="6">
+        <v>2</v>
+      </c>
+      <c r="G568" s="6">
+        <v>1</v>
+      </c>
+      <c r="H568" s="6">
+        <v>1</v>
+      </c>
+      <c r="I568" s="6">
+        <v>8</v>
+      </c>
+      <c r="J568" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="569" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A569" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B569" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C569" s="6">
+        <v>1</v>
+      </c>
+      <c r="D569" s="6">
+        <v>1</v>
+      </c>
+      <c r="E569" s="6">
+        <v>1</v>
+      </c>
+      <c r="F569" s="6">
+        <v>2</v>
+      </c>
+      <c r="G569" s="6">
+        <v>2</v>
+      </c>
+      <c r="H569" s="6">
+        <v>1</v>
+      </c>
+      <c r="I569" s="6">
+        <v>8</v>
+      </c>
+      <c r="J569" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="570" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A570" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B570" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C570" s="6">
+        <v>0</v>
+      </c>
+      <c r="D570" s="6">
+        <v>0</v>
+      </c>
+      <c r="E570" s="6">
+        <v>0</v>
+      </c>
+      <c r="F570" s="6">
+        <v>3</v>
+      </c>
+      <c r="G570" s="6">
+        <v>3</v>
+      </c>
+      <c r="H570" s="6">
+        <v>2</v>
+      </c>
+      <c r="I570" s="6">
+        <v>8</v>
+      </c>
+      <c r="J570" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="571" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A571" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B571" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C571" s="6">
+        <v>0</v>
+      </c>
+      <c r="D571" s="6">
+        <v>2</v>
+      </c>
+      <c r="E571" s="6">
+        <v>1</v>
+      </c>
+      <c r="F571" s="6">
+        <v>1</v>
+      </c>
+      <c r="G571" s="6">
+        <v>0</v>
+      </c>
+      <c r="H571" s="6">
+        <v>3</v>
+      </c>
+      <c r="I571" s="6">
+        <v>7</v>
+      </c>
+      <c r="J571" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="572" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A572" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B572" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C572" s="6">
+        <v>2</v>
+      </c>
+      <c r="D572" s="6">
+        <v>0</v>
+      </c>
+      <c r="E572" s="6">
+        <v>2</v>
+      </c>
+      <c r="F572" s="6">
+        <v>0</v>
+      </c>
+      <c r="G572" s="6">
+        <v>0</v>
+      </c>
+      <c r="H572" s="6">
+        <v>4</v>
+      </c>
+      <c r="I572" s="6">
+        <v>8</v>
+      </c>
+      <c r="J572" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="573" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A573" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B573" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C573" s="6">
+        <v>2</v>
+      </c>
+      <c r="D573" s="6">
+        <v>1</v>
+      </c>
+      <c r="E573" s="6">
+        <v>2</v>
+      </c>
+      <c r="F573" s="6">
+        <v>1</v>
+      </c>
+      <c r="G573" s="6">
+        <v>3</v>
+      </c>
+      <c r="H573" s="6">
+        <v>0</v>
+      </c>
+      <c r="I573" s="6">
+        <v>9</v>
+      </c>
+      <c r="J573" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="574" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A574" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B574" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C574" s="6">
+        <v>1</v>
+      </c>
+      <c r="D574" s="6">
+        <v>0</v>
+      </c>
+      <c r="E574" s="6">
+        <v>1</v>
+      </c>
+      <c r="F574" s="6">
+        <v>0</v>
+      </c>
+      <c r="G574" s="6">
+        <v>3</v>
+      </c>
+      <c r="H574" s="6">
+        <v>2</v>
+      </c>
+      <c r="I574" s="6">
+        <v>7</v>
+      </c>
+      <c r="J574" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="575" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A575" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B575" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C575" s="6">
+        <v>1</v>
+      </c>
+      <c r="D575" s="6">
+        <v>1</v>
+      </c>
+      <c r="E575" s="6">
+        <v>3</v>
+      </c>
+      <c r="F575" s="6">
+        <v>2</v>
+      </c>
+      <c r="G575" s="6">
+        <v>1</v>
+      </c>
+      <c r="H575" s="6">
+        <v>0</v>
+      </c>
+      <c r="I575" s="6">
+        <v>8</v>
+      </c>
+      <c r="J575" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A576" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B576" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C576" s="6">
+        <v>1</v>
+      </c>
+      <c r="D576" s="6">
+        <v>1</v>
+      </c>
+      <c r="E576" s="6">
+        <v>2</v>
+      </c>
+      <c r="F576" s="6">
+        <v>1</v>
+      </c>
+      <c r="G576" s="6">
+        <v>0</v>
+      </c>
+      <c r="H576" s="6">
+        <v>3</v>
+      </c>
+      <c r="I576" s="6">
+        <v>8</v>
+      </c>
+      <c r="J576" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="577" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A577" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B577" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C577" s="6">
+        <v>0</v>
+      </c>
+      <c r="D577" s="6">
+        <v>2</v>
+      </c>
+      <c r="E577" s="6">
+        <v>1</v>
+      </c>
+      <c r="F577" s="6">
+        <v>0</v>
+      </c>
+      <c r="G577" s="6">
+        <v>3</v>
+      </c>
+      <c r="H577" s="6">
+        <v>1</v>
+      </c>
+      <c r="I577" s="6">
+        <v>7</v>
+      </c>
+      <c r="J577" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="578" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A578" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B578" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C578" s="6">
+        <v>0</v>
+      </c>
+      <c r="D578" s="6">
+        <v>1</v>
+      </c>
+      <c r="E578" s="6">
+        <v>2</v>
+      </c>
+      <c r="F578" s="6">
+        <v>2</v>
+      </c>
+      <c r="G578" s="6">
+        <v>1</v>
+      </c>
+      <c r="H578" s="6">
+        <v>1</v>
+      </c>
+      <c r="I578" s="6">
+        <v>7</v>
+      </c>
+      <c r="J578" s="6">
+        <v>5</v>
+      </c>
+      <c r="K578" t="s">
+        <v>3</v>
+      </c>
+      <c r="L578" t="s">
+        <v>1</v>
+      </c>
+      <c r="M578">
         <v>12</v>
       </c>
-      <c r="N545">
+      <c r="N578">
         <v>158</v>
       </c>
-      <c r="O545">
-        <v>0</v>
+      <c r="O578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A579" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B579" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C579" s="6">
+        <v>0</v>
+      </c>
+      <c r="D579" s="6">
+        <v>1</v>
+      </c>
+      <c r="E579" s="6">
+        <v>4</v>
+      </c>
+      <c r="F579" s="6">
+        <v>1</v>
+      </c>
+      <c r="G579" s="6">
+        <v>1</v>
+      </c>
+      <c r="H579" s="6">
+        <v>1</v>
+      </c>
+      <c r="I579">
+        <v>8</v>
+      </c>
+      <c r="J579" s="6">
+        <v>5</v>
+      </c>
+      <c r="K579" t="s">
+        <v>3</v>
+      </c>
+      <c r="L579" t="s">
+        <v>1</v>
+      </c>
+      <c r="M579">
+        <v>12</v>
+      </c>
+      <c r="N579">
+        <v>158</v>
+      </c>
+      <c r="O579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A580" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B580" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C580" s="6">
+        <v>1</v>
+      </c>
+      <c r="D580" s="6">
+        <v>1</v>
+      </c>
+      <c r="E580" s="6">
+        <v>0</v>
+      </c>
+      <c r="F580" s="6">
+        <v>2</v>
+      </c>
+      <c r="G580" s="6">
+        <v>1</v>
+      </c>
+      <c r="H580" s="6">
+        <v>2</v>
+      </c>
+      <c r="I580">
+        <v>7</v>
+      </c>
+      <c r="J580" s="6">
+        <v>5</v>
+      </c>
+      <c r="K580" t="s">
+        <v>3</v>
+      </c>
+      <c r="L580" t="s">
+        <v>1</v>
+      </c>
+      <c r="M580">
+        <v>12</v>
+      </c>
+      <c r="N580">
+        <v>156</v>
+      </c>
+      <c r="O580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A581" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B581" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C581" s="6">
+        <v>0</v>
+      </c>
+      <c r="D581" s="6">
+        <v>3</v>
+      </c>
+      <c r="E581" s="6">
+        <v>2</v>
+      </c>
+      <c r="F581" s="6">
+        <v>1</v>
+      </c>
+      <c r="G581" s="6">
+        <v>1</v>
+      </c>
+      <c r="H581" s="6">
+        <v>0</v>
+      </c>
+      <c r="I581">
+        <v>7</v>
+      </c>
+      <c r="J581" s="6">
+        <v>4</v>
+      </c>
+      <c r="K581" t="s">
+        <v>3</v>
+      </c>
+      <c r="L581" t="s">
+        <v>1</v>
+      </c>
+      <c r="M581">
+        <v>12</v>
+      </c>
+      <c r="N581">
+        <v>158</v>
+      </c>
+      <c r="O581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A582" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B582" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C582" s="6">
+        <v>2</v>
+      </c>
+      <c r="D582" s="6">
+        <v>2</v>
+      </c>
+      <c r="E582" s="6">
+        <v>2</v>
+      </c>
+      <c r="F582" s="6">
+        <v>0</v>
+      </c>
+      <c r="G582" s="6">
+        <v>0</v>
+      </c>
+      <c r="H582" s="6">
+        <v>1</v>
+      </c>
+      <c r="I582">
+        <v>7</v>
+      </c>
+      <c r="J582" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="583" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A583" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B583" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C583" s="6">
+        <v>1</v>
+      </c>
+      <c r="D583" s="6">
+        <v>1</v>
+      </c>
+      <c r="E583" s="6">
+        <v>1</v>
+      </c>
+      <c r="F583" s="6">
+        <v>1</v>
+      </c>
+      <c r="G583" s="6">
+        <v>2</v>
+      </c>
+      <c r="H583" s="6">
+        <v>3</v>
+      </c>
+      <c r="I583">
+        <v>9</v>
+      </c>
+      <c r="J583" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="584" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A584" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B584" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C584" s="6">
+        <v>2</v>
+      </c>
+      <c r="D584" s="6">
+        <v>0</v>
+      </c>
+      <c r="E584" s="6">
+        <v>1</v>
+      </c>
+      <c r="F584" s="6">
+        <v>3</v>
+      </c>
+      <c r="G584" s="6">
+        <v>2</v>
+      </c>
+      <c r="H584" s="6">
+        <v>0</v>
+      </c>
+      <c r="I584">
+        <v>8</v>
+      </c>
+      <c r="J584" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="585" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A585" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B585" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C585" s="6">
+        <v>1</v>
+      </c>
+      <c r="D585" s="6">
+        <v>1</v>
+      </c>
+      <c r="E585" s="6">
+        <v>1</v>
+      </c>
+      <c r="F585" s="6">
+        <v>3</v>
+      </c>
+      <c r="G585" s="6">
+        <v>1</v>
+      </c>
+      <c r="H585" s="6">
+        <v>1</v>
+      </c>
+      <c r="I585">
+        <v>8</v>
+      </c>
+      <c r="J585" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="586" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A586" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B586" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C586" s="6">
+        <v>1</v>
+      </c>
+      <c r="D586" s="6">
+        <v>0</v>
+      </c>
+      <c r="E586" s="6">
+        <v>2</v>
+      </c>
+      <c r="F586" s="6">
+        <v>1</v>
+      </c>
+      <c r="G586" s="6">
+        <v>3</v>
+      </c>
+      <c r="H586" s="6">
+        <v>1</v>
+      </c>
+      <c r="I586">
+        <v>8</v>
+      </c>
+      <c r="J586" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="587" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A587" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B587" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C587" s="6">
+        <v>0</v>
+      </c>
+      <c r="D587" s="6">
+        <v>1</v>
+      </c>
+      <c r="E587" s="6">
+        <v>1</v>
+      </c>
+      <c r="F587" s="6">
+        <v>3</v>
+      </c>
+      <c r="G587" s="6">
+        <v>2</v>
+      </c>
+      <c r="H587" s="6">
+        <v>0</v>
+      </c>
+      <c r="I587">
+        <v>7</v>
+      </c>
+      <c r="J587" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="588" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A588" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B588" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C588" s="6">
+        <v>1</v>
+      </c>
+      <c r="D588" s="6">
+        <v>2</v>
+      </c>
+      <c r="E588" s="6">
+        <v>2</v>
+      </c>
+      <c r="F588" s="6">
+        <v>3</v>
+      </c>
+      <c r="G588" s="6">
+        <v>1</v>
+      </c>
+      <c r="H588" s="6">
+        <v>1</v>
+      </c>
+      <c r="I588">
+        <v>10</v>
+      </c>
+      <c r="J588" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="589" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A589" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B589" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C589" s="6">
+        <v>3</v>
+      </c>
+      <c r="D589" s="6">
+        <v>4</v>
+      </c>
+      <c r="E589" s="6">
+        <v>1</v>
+      </c>
+      <c r="F589" s="6">
+        <v>0</v>
+      </c>
+      <c r="G589" s="6">
+        <v>0</v>
+      </c>
+      <c r="H589" s="6">
+        <v>2</v>
+      </c>
+      <c r="I589">
+        <v>10</v>
+      </c>
+      <c r="J589" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="590" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A590" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B590" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C590" s="6">
+        <v>1</v>
+      </c>
+      <c r="D590" s="6">
+        <v>1</v>
+      </c>
+      <c r="E590" s="6">
+        <v>1</v>
+      </c>
+      <c r="F590" s="6">
+        <v>2</v>
+      </c>
+      <c r="G590" s="6">
+        <v>2</v>
+      </c>
+      <c r="H590" s="6">
+        <v>1</v>
+      </c>
+      <c r="I590">
+        <v>8</v>
+      </c>
+      <c r="J590" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="591" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A591" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B591" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C591" s="6">
+        <v>2</v>
+      </c>
+      <c r="D591" s="6">
+        <v>1</v>
+      </c>
+      <c r="E591" s="6">
+        <v>1</v>
+      </c>
+      <c r="F591" s="6">
+        <v>1</v>
+      </c>
+      <c r="G591" s="6">
+        <v>2</v>
+      </c>
+      <c r="H591" s="6">
+        <v>3</v>
+      </c>
+      <c r="I591">
+        <v>10</v>
+      </c>
+      <c r="J591" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="592" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A592" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B592" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C592" s="6">
+        <v>2</v>
+      </c>
+      <c r="D592" s="6">
+        <v>1</v>
+      </c>
+      <c r="E592" s="6">
+        <v>1</v>
+      </c>
+      <c r="F592" s="6">
+        <v>3</v>
+      </c>
+      <c r="G592" s="6">
+        <v>1</v>
+      </c>
+      <c r="H592" s="6">
+        <v>1</v>
+      </c>
+      <c r="I592">
+        <v>9</v>
+      </c>
+      <c r="J592" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="593" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A593" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B593" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C593" s="6">
+        <v>0</v>
+      </c>
+      <c r="D593" s="6">
+        <v>2</v>
+      </c>
+      <c r="E593" s="6">
+        <v>1</v>
+      </c>
+      <c r="F593" s="6">
+        <v>2</v>
+      </c>
+      <c r="G593" s="6">
+        <v>4</v>
+      </c>
+      <c r="H593" s="6">
+        <v>0</v>
+      </c>
+      <c r="I593">
+        <v>9</v>
+      </c>
+      <c r="J593" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A594" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B594" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C594" s="6">
+        <v>1</v>
+      </c>
+      <c r="D594" s="6">
+        <v>2</v>
+      </c>
+      <c r="E594" s="6">
+        <v>0</v>
+      </c>
+      <c r="F594" s="6">
+        <v>0</v>
+      </c>
+      <c r="G594" s="6">
+        <v>2</v>
+      </c>
+      <c r="H594" s="6">
+        <v>3</v>
+      </c>
+      <c r="I594">
+        <v>9</v>
+      </c>
+      <c r="J594" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A595" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B595" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C595" s="6">
+        <v>0</v>
+      </c>
+      <c r="D595" s="6">
+        <v>3</v>
+      </c>
+      <c r="E595" s="6">
+        <v>2</v>
+      </c>
+      <c r="F595" s="6">
+        <v>1</v>
+      </c>
+      <c r="G595" s="6">
+        <v>2</v>
+      </c>
+      <c r="H595" s="6">
+        <v>0</v>
+      </c>
+      <c r="I595">
+        <v>8</v>
+      </c>
+      <c r="J595" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A596" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B596" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C596" s="6">
+        <v>0</v>
+      </c>
+      <c r="D596">
+        <v>0</v>
+      </c>
+      <c r="E596">
+        <v>0</v>
+      </c>
+      <c r="F596">
+        <v>4</v>
+      </c>
+      <c r="G596">
+        <v>2</v>
+      </c>
+      <c r="H596">
+        <v>2</v>
+      </c>
+      <c r="I596">
+        <v>8</v>
+      </c>
+      <c r="J596" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A597" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B597" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C597" s="6">
+        <v>0</v>
+      </c>
+      <c r="D597">
+        <v>0</v>
+      </c>
+      <c r="E597">
+        <v>1</v>
+      </c>
+      <c r="F597">
+        <v>2</v>
+      </c>
+      <c r="G597">
+        <v>4</v>
+      </c>
+      <c r="H597">
+        <v>1</v>
+      </c>
+      <c r="I597">
+        <v>8</v>
+      </c>
+      <c r="J597" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A598" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B598" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C598" s="6">
+        <v>0</v>
+      </c>
+      <c r="D598">
+        <v>0</v>
+      </c>
+      <c r="E598">
+        <v>4</v>
+      </c>
+      <c r="F598">
+        <v>2</v>
+      </c>
+      <c r="G598">
+        <v>1</v>
+      </c>
+      <c r="H598">
+        <v>1</v>
+      </c>
+      <c r="I598">
+        <v>8</v>
+      </c>
+      <c r="J598" s="6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>